<commit_message>
2016 metadata link update
</commit_message>
<xml_diff>
--- a/static/download/2016/RP2_APT_ATC_PRE_2016.xlsx
+++ b/static/download/2016/RP2_APT_ATC_PRE_2016.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="APT_ATC_PRE_LOC" sheetId="1" r:id="rId3"/>
@@ -27,7 +27,7 @@
     <t>Meta data</t>
   </si>
   <si>
-    <t>ATC pre-departure delay</t>
+    <t>Metadata - Single European Sky Portal</t>
   </si>
   <si>
     <t>Release date</t>
@@ -42,7 +42,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>NSA-PRU-Support@eurocontrol.int</t>
+    <t>pru-support@eurocontrol.int</t>
   </si>
   <si>
     <t>Period: JAN-DEC</t>
@@ -381,6 +381,879 @@
     <t>London/ Gatwick</t>
   </si>
   <si>
+    <t>EGKK</t>
+  </si>
+  <si>
+    <t>London/ City</t>
+  </si>
+  <si>
+    <t>EGLC</t>
+  </si>
+  <si>
+    <t>London/ Heathrow</t>
+  </si>
+  <si>
+    <t>EGLL</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>EGPF</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>EGPH</t>
+  </si>
+  <si>
+    <t>London/ Stansted</t>
+  </si>
+  <si>
+    <t>EGSS</t>
+  </si>
+  <si>
+    <t>Amsterdam/ Schiphol</t>
+  </si>
+  <si>
+    <t>EHAM</t>
+  </si>
+  <si>
+    <t>Maastricht-Aachen</t>
+  </si>
+  <si>
+    <t>EHBK</t>
+  </si>
+  <si>
+    <t>Groningen</t>
+  </si>
+  <si>
+    <t>EHGG</t>
+  </si>
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>EHRD</t>
+  </si>
+  <si>
+    <t>Cork</t>
+  </si>
+  <si>
+    <t>EICK</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>EIDW</t>
+  </si>
+  <si>
+    <t>Shannon</t>
+  </si>
+  <si>
+    <t>EINN</t>
+  </si>
+  <si>
+    <t>Copenhagen/ Kastrup</t>
+  </si>
+  <si>
+    <t>EKCH</t>
+  </si>
+  <si>
+    <t>ELLX</t>
+  </si>
+  <si>
+    <t>Bergen</t>
+  </si>
+  <si>
+    <t>ENBR</t>
+  </si>
+  <si>
+    <t>Oslo/ Gardermoen</t>
+  </si>
+  <si>
+    <t>ENGM</t>
+  </si>
+  <si>
+    <t>Trondheim</t>
+  </si>
+  <si>
+    <t>ENVA</t>
+  </si>
+  <si>
+    <t>Stavanger</t>
+  </si>
+  <si>
+    <t>ENZV</t>
+  </si>
+  <si>
+    <t>Bydgoszcz</t>
+  </si>
+  <si>
+    <t>EPBY</t>
+  </si>
+  <si>
+    <t>Gdansk</t>
+  </si>
+  <si>
+    <t>EPGD</t>
+  </si>
+  <si>
+    <t>Krakow - Balice</t>
+  </si>
+  <si>
+    <t>EPKK</t>
+  </si>
+  <si>
+    <t>Katowice - Pyrzowice</t>
+  </si>
+  <si>
+    <t>EPKT</t>
+  </si>
+  <si>
+    <t>Lublin</t>
+  </si>
+  <si>
+    <t>EPLB</t>
+  </si>
+  <si>
+    <t>Lodz - Lublinek</t>
+  </si>
+  <si>
+    <t>EPLL</t>
+  </si>
+  <si>
+    <t>Warszawa/ Modlin</t>
+  </si>
+  <si>
+    <t>EPMO</t>
+  </si>
+  <si>
+    <t>Poznan - Lawica</t>
+  </si>
+  <si>
+    <t>EPPO</t>
+  </si>
+  <si>
+    <t>Radom</t>
+  </si>
+  <si>
+    <t>EPRA</t>
+  </si>
+  <si>
+    <t>Rzeszow - Jasionka</t>
+  </si>
+  <si>
+    <t>EPRZ</t>
+  </si>
+  <si>
+    <t>Szczecin - Goleniów</t>
+  </si>
+  <si>
+    <t>EPSC</t>
+  </si>
+  <si>
+    <t>Olsztyn-Mazury</t>
+  </si>
+  <si>
+    <t>EPSY</t>
+  </si>
+  <si>
+    <t>Warszawa/ Chopina</t>
+  </si>
+  <si>
+    <t>EPWA</t>
+  </si>
+  <si>
+    <t>Wroclaw/ Strachowice</t>
+  </si>
+  <si>
+    <t>EPWR</t>
+  </si>
+  <si>
+    <t>Zielona Gora - Babimost</t>
+  </si>
+  <si>
+    <t>EPZG</t>
+  </si>
+  <si>
+    <t>Stockholm/ Arlanda</t>
+  </si>
+  <si>
+    <t>ESSA</t>
+  </si>
+  <si>
+    <t>Liepaja</t>
+  </si>
+  <si>
+    <t>EVLA</t>
+  </si>
+  <si>
+    <t>Riga</t>
+  </si>
+  <si>
+    <t>EVRA</t>
+  </si>
+  <si>
+    <t>Ventspils</t>
+  </si>
+  <si>
+    <t>EVVA</t>
+  </si>
+  <si>
+    <t>Kaunas</t>
+  </si>
+  <si>
+    <t>EYKA</t>
+  </si>
+  <si>
+    <t>Palanga</t>
+  </si>
+  <si>
+    <t>EYPA</t>
+  </si>
+  <si>
+    <t>Šiauliai</t>
+  </si>
+  <si>
+    <t>EYSA</t>
+  </si>
+  <si>
+    <t>Vilnius</t>
+  </si>
+  <si>
+    <t>EYVI</t>
+  </si>
+  <si>
+    <t>Gran Canaria</t>
+  </si>
+  <si>
+    <t>GCLP</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>LBSF</t>
+  </si>
+  <si>
+    <t>Larnaca</t>
+  </si>
+  <si>
+    <t>LCLK</t>
+  </si>
+  <si>
+    <t>Paphos</t>
+  </si>
+  <si>
+    <t>LCPH</t>
+  </si>
+  <si>
+    <t>Zagreb</t>
+  </si>
+  <si>
+    <t>LDZA</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>LEBL</t>
+  </si>
+  <si>
+    <t>Madrid/ Barajas</t>
+  </si>
+  <si>
+    <t>LEMD</t>
+  </si>
+  <si>
+    <t>Málaga</t>
+  </si>
+  <si>
+    <t>LEMG</t>
+  </si>
+  <si>
+    <t>Palma de Mallorca</t>
+  </si>
+  <si>
+    <t>LEPA</t>
+  </si>
+  <si>
+    <t>Albert-Bray</t>
+  </si>
+  <si>
+    <t>LFAQ</t>
+  </si>
+  <si>
+    <t>Agen-La Garenne</t>
+  </si>
+  <si>
+    <t>LFBA</t>
+  </si>
+  <si>
+    <t>Bordeaux-Mérignac</t>
+  </si>
+  <si>
+    <t>LFBD</t>
+  </si>
+  <si>
+    <t>Bergerac-Roumanière</t>
+  </si>
+  <si>
+    <t>LFBE</t>
+  </si>
+  <si>
+    <t>La Rochelle-Ile de Ré</t>
+  </si>
+  <si>
+    <t>LFBH</t>
+  </si>
+  <si>
+    <t>Poitiers-Biard</t>
+  </si>
+  <si>
+    <t>LFBI</t>
+  </si>
+  <si>
+    <t>Limoges-Bellegarde</t>
+  </si>
+  <si>
+    <t>LFBL</t>
+  </si>
+  <si>
+    <t>Toulouse-Blagnac</t>
+  </si>
+  <si>
+    <t>LFBO</t>
+  </si>
+  <si>
+    <t>Pau-Pyrénées</t>
+  </si>
+  <si>
+    <t>LFBP</t>
+  </si>
+  <si>
+    <t>Tarbes-Lourdes Pyrénées</t>
+  </si>
+  <si>
+    <t>LFBT</t>
+  </si>
+  <si>
+    <t>Biarritz-Bayonne-Anglet</t>
+  </si>
+  <si>
+    <t>LFBZ</t>
+  </si>
+  <si>
+    <t>Rodez-Marcillac</t>
+  </si>
+  <si>
+    <t>LFCR</t>
+  </si>
+  <si>
+    <t>Dôle-Tavaux</t>
+  </si>
+  <si>
+    <t>LFGJ</t>
+  </si>
+  <si>
+    <t>Metz-Nancy-Lorraine</t>
+  </si>
+  <si>
+    <t>LFJL</t>
+  </si>
+  <si>
+    <t>Angers-Marcé</t>
+  </si>
+  <si>
+    <t>LFJR</t>
+  </si>
+  <si>
+    <t>Bastia-Poretta</t>
+  </si>
+  <si>
+    <t>LFKB</t>
+  </si>
+  <si>
+    <t>Calvi-Sainte-Catherine</t>
+  </si>
+  <si>
+    <t>LFKC</t>
+  </si>
+  <si>
+    <t>Figari-Sud Corse</t>
+  </si>
+  <si>
+    <t>LFKF</t>
+  </si>
+  <si>
+    <t>Ajaccio-Napoléon-Bonaparte</t>
+  </si>
+  <si>
+    <t>LFKJ</t>
+  </si>
+  <si>
+    <t>Chambéry-Aix-les-Bains</t>
+  </si>
+  <si>
+    <t>LFLB</t>
+  </si>
+  <si>
+    <t>Clermont-Ferrand-Auvergne</t>
+  </si>
+  <si>
+    <t>LFLC</t>
+  </si>
+  <si>
+    <t>Lyon-Saint-Exupéry</t>
+  </si>
+  <si>
+    <t>LFLL</t>
+  </si>
+  <si>
+    <t>Annecy-Meythet</t>
+  </si>
+  <si>
+    <t>LFLP</t>
+  </si>
+  <si>
+    <t>Grenoble-Isère</t>
+  </si>
+  <si>
+    <t>LFLS</t>
+  </si>
+  <si>
+    <t>Châteauroux-Déols</t>
+  </si>
+  <si>
+    <t>LFLX</t>
+  </si>
+  <si>
+    <t>Lyon-Bron</t>
+  </si>
+  <si>
+    <t>LFLY</t>
+  </si>
+  <si>
+    <t>Cannes-Mandelieu</t>
+  </si>
+  <si>
+    <t>LFMD</t>
+  </si>
+  <si>
+    <t>Saint-Etienne-Bouthéon</t>
+  </si>
+  <si>
+    <t>LFMH</t>
+  </si>
+  <si>
+    <t>Istres-Le Tubé</t>
+  </si>
+  <si>
+    <t>LFMI</t>
+  </si>
+  <si>
+    <t>Carcassonne-Salvaza</t>
+  </si>
+  <si>
+    <t>LFMK</t>
+  </si>
+  <si>
+    <t>Marseille-Provence</t>
+  </si>
+  <si>
+    <t>LFML</t>
+  </si>
+  <si>
+    <t>Nice-Côte d’Azur</t>
+  </si>
+  <si>
+    <t>LFMN</t>
+  </si>
+  <si>
+    <t>Perpignan-Rivesaltes</t>
+  </si>
+  <si>
+    <t>LFMP</t>
+  </si>
+  <si>
+    <t>Montpellier-Méditerranée</t>
+  </si>
+  <si>
+    <t>LFMT</t>
+  </si>
+  <si>
+    <t>Béziers-Vias</t>
+  </si>
+  <si>
+    <t>LFMU</t>
+  </si>
+  <si>
+    <t>Avignon-Caumont</t>
+  </si>
+  <si>
+    <t>LFMV</t>
+  </si>
+  <si>
+    <t>Beauvais-Tillé</t>
+  </si>
+  <si>
+    <t>LFOB</t>
+  </si>
+  <si>
+    <t>Le Havre-Octeville</t>
+  </si>
+  <si>
+    <t>LFOH</t>
+  </si>
+  <si>
+    <t>Châlons-Vatry</t>
+  </si>
+  <si>
+    <t>LFOK</t>
+  </si>
+  <si>
+    <t>Tours-Val de Loire</t>
+  </si>
+  <si>
+    <t>LFOT</t>
+  </si>
+  <si>
+    <t>Paris-Le Bourget</t>
+  </si>
+  <si>
+    <t>LFPB</t>
+  </si>
+  <si>
+    <t>Paris-Charles-de-Gaulle</t>
+  </si>
+  <si>
+    <t>LFPG</t>
+  </si>
+  <si>
+    <t>Toussus-le-Noble</t>
+  </si>
+  <si>
+    <t>LFPN</t>
+  </si>
+  <si>
+    <t>Paris-Orly</t>
+  </si>
+  <si>
+    <t>LFPO</t>
+  </si>
+  <si>
+    <t>Lille-Lesquin</t>
+  </si>
+  <si>
+    <t>LFQQ</t>
+  </si>
+  <si>
+    <t>Brest-Bretagne</t>
+  </si>
+  <si>
+    <t>LFRB</t>
+  </si>
+  <si>
+    <t>Dinard-Pleurtuit-Saint-Malo</t>
+  </si>
+  <si>
+    <t>LFRD</t>
+  </si>
+  <si>
+    <t>Deauville-Normandie</t>
+  </si>
+  <si>
+    <t>LFRG</t>
+  </si>
+  <si>
+    <t>Lorient-Lann Bihoué</t>
+  </si>
+  <si>
+    <t>LFRH</t>
+  </si>
+  <si>
+    <t>Caen-Carpiquet</t>
+  </si>
+  <si>
+    <t>LFRK</t>
+  </si>
+  <si>
+    <t>Rennes-Saint-Jacques</t>
+  </si>
+  <si>
+    <t>LFRN</t>
+  </si>
+  <si>
+    <t>Lannion</t>
+  </si>
+  <si>
+    <t>LFRO</t>
+  </si>
+  <si>
+    <t>Quimper-Pluguffan</t>
+  </si>
+  <si>
+    <t>LFRQ</t>
+  </si>
+  <si>
+    <t>Nantes-Atlantique</t>
+  </si>
+  <si>
+    <t>LFRS</t>
+  </si>
+  <si>
+    <t>Saint-Nazaire-Montoir</t>
+  </si>
+  <si>
+    <t>LFRZ</t>
+  </si>
+  <si>
+    <t>Bâle-Mulhouse</t>
+  </si>
+  <si>
+    <t>LFSB</t>
+  </si>
+  <si>
+    <t>Brive-Souillac</t>
+  </si>
+  <si>
+    <t>LFSL</t>
+  </si>
+  <si>
+    <t>Strasbourg-Entzheim</t>
+  </si>
+  <si>
+    <t>LFST</t>
+  </si>
+  <si>
+    <t>Hyères-Le Palyvestre</t>
+  </si>
+  <si>
+    <t>LFTH</t>
+  </si>
+  <si>
+    <t>Nîmes-Garons</t>
+  </si>
+  <si>
+    <t>LFTW</t>
+  </si>
+  <si>
+    <t>Athens</t>
+  </si>
+  <si>
+    <t>LGAV</t>
+  </si>
+  <si>
+    <t>Budapest/ Ferihegy</t>
+  </si>
+  <si>
+    <t>LHBP</t>
+  </si>
+  <si>
+    <t>Milan/ Malpensa</t>
+  </si>
+  <si>
+    <t>LIMC</t>
+  </si>
+  <si>
+    <t>Bergamo</t>
+  </si>
+  <si>
+    <t>LIME</t>
+  </si>
+  <si>
+    <t>Milan/ Linate</t>
+  </si>
+  <si>
+    <t>LIML</t>
+  </si>
+  <si>
+    <t>Venice</t>
+  </si>
+  <si>
+    <t>LIPZ</t>
+  </si>
+  <si>
+    <t>Rome/Fiumicino</t>
+  </si>
+  <si>
+    <t>LIRF</t>
+  </si>
+  <si>
+    <t>Ljubljana</t>
+  </si>
+  <si>
+    <t>LJLJ</t>
+  </si>
+  <si>
+    <t>Maribor</t>
+  </si>
+  <si>
+    <t>LJMB</t>
+  </si>
+  <si>
+    <t>Portorož</t>
+  </si>
+  <si>
+    <t>LJPZ</t>
+  </si>
+  <si>
+    <t>Karlovy Vary</t>
+  </si>
+  <si>
+    <t>LKKV</t>
+  </si>
+  <si>
+    <t>Ostrava</t>
+  </si>
+  <si>
+    <t>LKMT</t>
+  </si>
+  <si>
+    <t>Prague</t>
+  </si>
+  <si>
+    <t>LKPR</t>
+  </si>
+  <si>
+    <t>Brno-Tuřany</t>
+  </si>
+  <si>
+    <t>LKTB</t>
+  </si>
+  <si>
+    <t>LMML</t>
+  </si>
+  <si>
+    <t>Graz</t>
+  </si>
+  <si>
+    <t>LOWG</t>
+  </si>
+  <si>
+    <t>Innsbruck</t>
+  </si>
+  <si>
+    <t>LOWI</t>
+  </si>
+  <si>
+    <t>Klagenfurt</t>
+  </si>
+  <si>
+    <t>LOWK</t>
+  </si>
+  <si>
+    <t>Linz</t>
+  </si>
+  <si>
+    <t>LOWL</t>
+  </si>
+  <si>
+    <t>Salzburg</t>
+  </si>
+  <si>
+    <t>LOWS</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>LOWW</t>
+  </si>
+  <si>
+    <t>Santa Maria</t>
+  </si>
+  <si>
+    <t>LPAZ</t>
+  </si>
+  <si>
+    <t>Cascais</t>
+  </si>
+  <si>
+    <t>LPCS</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>LPFL</t>
+  </si>
+  <si>
+    <t>Faro</t>
+  </si>
+  <si>
+    <t>LPFR</t>
+  </si>
+  <si>
+    <t>Horta</t>
+  </si>
+  <si>
+    <t>LPHR</t>
+  </si>
+  <si>
+    <t>Madeira</t>
+  </si>
+  <si>
+    <t>LPMA</t>
+  </si>
+  <si>
+    <t>Ponta Delgada</t>
+  </si>
+  <si>
+    <t>LPPD</t>
+  </si>
+  <si>
+    <t>Porto</t>
+  </si>
+  <si>
+    <t>LPPR</t>
+  </si>
+  <si>
+    <t>Porto Santo</t>
+  </si>
+  <si>
+    <t>LPPS</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>LPPT</t>
+  </si>
+  <si>
+    <t>Bucharest/ Băneasa</t>
+  </si>
+  <si>
+    <t>LRBS</t>
+  </si>
+  <si>
+    <t>Bucharest/ Otopeni</t>
+  </si>
+  <si>
+    <t>LROP</t>
+  </si>
+  <si>
+    <t>Geneva</t>
+  </si>
+  <si>
+    <t>LSGG</t>
+  </si>
+  <si>
+    <t>Zürich</t>
+  </si>
+  <si>
+    <t>LSZH</t>
+  </si>
+  <si>
+    <t>Bratislava</t>
+  </si>
+  <si>
+    <t>LZIB</t>
+  </si>
+  <si>
     <t>Change date</t>
   </si>
   <si>
@@ -409,879 +1282,6 @@
   </si>
   <si>
     <t>Data revisions based on further validations and additional data received</t>
-  </si>
-  <si>
-    <t>EGKK</t>
-  </si>
-  <si>
-    <t>London/ City</t>
-  </si>
-  <si>
-    <t>EGLC</t>
-  </si>
-  <si>
-    <t>London/ Heathrow</t>
-  </si>
-  <si>
-    <t>EGLL</t>
-  </si>
-  <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>EGPF</t>
-  </si>
-  <si>
-    <t>Edinburgh</t>
-  </si>
-  <si>
-    <t>EGPH</t>
-  </si>
-  <si>
-    <t>London/ Stansted</t>
-  </si>
-  <si>
-    <t>EGSS</t>
-  </si>
-  <si>
-    <t>Amsterdam/ Schiphol</t>
-  </si>
-  <si>
-    <t>EHAM</t>
-  </si>
-  <si>
-    <t>Maastricht-Aachen</t>
-  </si>
-  <si>
-    <t>EHBK</t>
-  </si>
-  <si>
-    <t>Groningen</t>
-  </si>
-  <si>
-    <t>EHGG</t>
-  </si>
-  <si>
-    <t>Rotterdam</t>
-  </si>
-  <si>
-    <t>EHRD</t>
-  </si>
-  <si>
-    <t>Cork</t>
-  </si>
-  <si>
-    <t>EICK</t>
-  </si>
-  <si>
-    <t>Dublin</t>
-  </si>
-  <si>
-    <t>EIDW</t>
-  </si>
-  <si>
-    <t>Shannon</t>
-  </si>
-  <si>
-    <t>EINN</t>
-  </si>
-  <si>
-    <t>Copenhagen/ Kastrup</t>
-  </si>
-  <si>
-    <t>EKCH</t>
-  </si>
-  <si>
-    <t>ELLX</t>
-  </si>
-  <si>
-    <t>Bergen</t>
-  </si>
-  <si>
-    <t>ENBR</t>
-  </si>
-  <si>
-    <t>Oslo/ Gardermoen</t>
-  </si>
-  <si>
-    <t>ENGM</t>
-  </si>
-  <si>
-    <t>Trondheim</t>
-  </si>
-  <si>
-    <t>ENVA</t>
-  </si>
-  <si>
-    <t>Stavanger</t>
-  </si>
-  <si>
-    <t>ENZV</t>
-  </si>
-  <si>
-    <t>Bydgoszcz</t>
-  </si>
-  <si>
-    <t>EPBY</t>
-  </si>
-  <si>
-    <t>Gdansk</t>
-  </si>
-  <si>
-    <t>EPGD</t>
-  </si>
-  <si>
-    <t>Krakow - Balice</t>
-  </si>
-  <si>
-    <t>EPKK</t>
-  </si>
-  <si>
-    <t>Katowice - Pyrzowice</t>
-  </si>
-  <si>
-    <t>EPKT</t>
-  </si>
-  <si>
-    <t>Lublin</t>
-  </si>
-  <si>
-    <t>EPLB</t>
-  </si>
-  <si>
-    <t>Lodz - Lublinek</t>
-  </si>
-  <si>
-    <t>EPLL</t>
-  </si>
-  <si>
-    <t>Warszawa/ Modlin</t>
-  </si>
-  <si>
-    <t>EPMO</t>
-  </si>
-  <si>
-    <t>Poznan - Lawica</t>
-  </si>
-  <si>
-    <t>EPPO</t>
-  </si>
-  <si>
-    <t>Radom</t>
-  </si>
-  <si>
-    <t>EPRA</t>
-  </si>
-  <si>
-    <t>Rzeszow - Jasionka</t>
-  </si>
-  <si>
-    <t>EPRZ</t>
-  </si>
-  <si>
-    <t>Szczecin - Goleniów</t>
-  </si>
-  <si>
-    <t>EPSC</t>
-  </si>
-  <si>
-    <t>Olsztyn-Mazury</t>
-  </si>
-  <si>
-    <t>EPSY</t>
-  </si>
-  <si>
-    <t>Warszawa/ Chopina</t>
-  </si>
-  <si>
-    <t>EPWA</t>
-  </si>
-  <si>
-    <t>Wroclaw/ Strachowice</t>
-  </si>
-  <si>
-    <t>EPWR</t>
-  </si>
-  <si>
-    <t>Zielona Gora - Babimost</t>
-  </si>
-  <si>
-    <t>EPZG</t>
-  </si>
-  <si>
-    <t>Stockholm/ Arlanda</t>
-  </si>
-  <si>
-    <t>ESSA</t>
-  </si>
-  <si>
-    <t>Liepaja</t>
-  </si>
-  <si>
-    <t>EVLA</t>
-  </si>
-  <si>
-    <t>Riga</t>
-  </si>
-  <si>
-    <t>EVRA</t>
-  </si>
-  <si>
-    <t>Ventspils</t>
-  </si>
-  <si>
-    <t>EVVA</t>
-  </si>
-  <si>
-    <t>Kaunas</t>
-  </si>
-  <si>
-    <t>EYKA</t>
-  </si>
-  <si>
-    <t>Palanga</t>
-  </si>
-  <si>
-    <t>EYPA</t>
-  </si>
-  <si>
-    <t>Šiauliai</t>
-  </si>
-  <si>
-    <t>EYSA</t>
-  </si>
-  <si>
-    <t>Vilnius</t>
-  </si>
-  <si>
-    <t>EYVI</t>
-  </si>
-  <si>
-    <t>Gran Canaria</t>
-  </si>
-  <si>
-    <t>GCLP</t>
-  </si>
-  <si>
-    <t>Sofia</t>
-  </si>
-  <si>
-    <t>LBSF</t>
-  </si>
-  <si>
-    <t>Larnaca</t>
-  </si>
-  <si>
-    <t>LCLK</t>
-  </si>
-  <si>
-    <t>Paphos</t>
-  </si>
-  <si>
-    <t>LCPH</t>
-  </si>
-  <si>
-    <t>Zagreb</t>
-  </si>
-  <si>
-    <t>LDZA</t>
-  </si>
-  <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
-    <t>LEBL</t>
-  </si>
-  <si>
-    <t>Madrid/ Barajas</t>
-  </si>
-  <si>
-    <t>LEMD</t>
-  </si>
-  <si>
-    <t>Málaga</t>
-  </si>
-  <si>
-    <t>LEMG</t>
-  </si>
-  <si>
-    <t>Palma de Mallorca</t>
-  </si>
-  <si>
-    <t>LEPA</t>
-  </si>
-  <si>
-    <t>Albert-Bray</t>
-  </si>
-  <si>
-    <t>LFAQ</t>
-  </si>
-  <si>
-    <t>Agen-La Garenne</t>
-  </si>
-  <si>
-    <t>LFBA</t>
-  </si>
-  <si>
-    <t>Bordeaux-Mérignac</t>
-  </si>
-  <si>
-    <t>LFBD</t>
-  </si>
-  <si>
-    <t>Bergerac-Roumanière</t>
-  </si>
-  <si>
-    <t>LFBE</t>
-  </si>
-  <si>
-    <t>La Rochelle-Ile de Ré</t>
-  </si>
-  <si>
-    <t>LFBH</t>
-  </si>
-  <si>
-    <t>Poitiers-Biard</t>
-  </si>
-  <si>
-    <t>LFBI</t>
-  </si>
-  <si>
-    <t>Limoges-Bellegarde</t>
-  </si>
-  <si>
-    <t>LFBL</t>
-  </si>
-  <si>
-    <t>Toulouse-Blagnac</t>
-  </si>
-  <si>
-    <t>LFBO</t>
-  </si>
-  <si>
-    <t>Pau-Pyrénées</t>
-  </si>
-  <si>
-    <t>LFBP</t>
-  </si>
-  <si>
-    <t>Tarbes-Lourdes Pyrénées</t>
-  </si>
-  <si>
-    <t>LFBT</t>
-  </si>
-  <si>
-    <t>Biarritz-Bayonne-Anglet</t>
-  </si>
-  <si>
-    <t>LFBZ</t>
-  </si>
-  <si>
-    <t>Rodez-Marcillac</t>
-  </si>
-  <si>
-    <t>LFCR</t>
-  </si>
-  <si>
-    <t>Dôle-Tavaux</t>
-  </si>
-  <si>
-    <t>LFGJ</t>
-  </si>
-  <si>
-    <t>Metz-Nancy-Lorraine</t>
-  </si>
-  <si>
-    <t>LFJL</t>
-  </si>
-  <si>
-    <t>Angers-Marcé</t>
-  </si>
-  <si>
-    <t>LFJR</t>
-  </si>
-  <si>
-    <t>Bastia-Poretta</t>
-  </si>
-  <si>
-    <t>LFKB</t>
-  </si>
-  <si>
-    <t>Calvi-Sainte-Catherine</t>
-  </si>
-  <si>
-    <t>LFKC</t>
-  </si>
-  <si>
-    <t>Figari-Sud Corse</t>
-  </si>
-  <si>
-    <t>LFKF</t>
-  </si>
-  <si>
-    <t>Ajaccio-Napoléon-Bonaparte</t>
-  </si>
-  <si>
-    <t>LFKJ</t>
-  </si>
-  <si>
-    <t>Chambéry-Aix-les-Bains</t>
-  </si>
-  <si>
-    <t>LFLB</t>
-  </si>
-  <si>
-    <t>Clermont-Ferrand-Auvergne</t>
-  </si>
-  <si>
-    <t>LFLC</t>
-  </si>
-  <si>
-    <t>Lyon-Saint-Exupéry</t>
-  </si>
-  <si>
-    <t>LFLL</t>
-  </si>
-  <si>
-    <t>Annecy-Meythet</t>
-  </si>
-  <si>
-    <t>LFLP</t>
-  </si>
-  <si>
-    <t>Grenoble-Isère</t>
-  </si>
-  <si>
-    <t>LFLS</t>
-  </si>
-  <si>
-    <t>Châteauroux-Déols</t>
-  </si>
-  <si>
-    <t>LFLX</t>
-  </si>
-  <si>
-    <t>Lyon-Bron</t>
-  </si>
-  <si>
-    <t>LFLY</t>
-  </si>
-  <si>
-    <t>Cannes-Mandelieu</t>
-  </si>
-  <si>
-    <t>LFMD</t>
-  </si>
-  <si>
-    <t>Saint-Etienne-Bouthéon</t>
-  </si>
-  <si>
-    <t>LFMH</t>
-  </si>
-  <si>
-    <t>Istres-Le Tubé</t>
-  </si>
-  <si>
-    <t>LFMI</t>
-  </si>
-  <si>
-    <t>Carcassonne-Salvaza</t>
-  </si>
-  <si>
-    <t>LFMK</t>
-  </si>
-  <si>
-    <t>Marseille-Provence</t>
-  </si>
-  <si>
-    <t>LFML</t>
-  </si>
-  <si>
-    <t>Nice-Côte d’Azur</t>
-  </si>
-  <si>
-    <t>LFMN</t>
-  </si>
-  <si>
-    <t>Perpignan-Rivesaltes</t>
-  </si>
-  <si>
-    <t>LFMP</t>
-  </si>
-  <si>
-    <t>Montpellier-Méditerranée</t>
-  </si>
-  <si>
-    <t>LFMT</t>
-  </si>
-  <si>
-    <t>Béziers-Vias</t>
-  </si>
-  <si>
-    <t>LFMU</t>
-  </si>
-  <si>
-    <t>Avignon-Caumont</t>
-  </si>
-  <si>
-    <t>LFMV</t>
-  </si>
-  <si>
-    <t>Beauvais-Tillé</t>
-  </si>
-  <si>
-    <t>LFOB</t>
-  </si>
-  <si>
-    <t>Le Havre-Octeville</t>
-  </si>
-  <si>
-    <t>LFOH</t>
-  </si>
-  <si>
-    <t>Châlons-Vatry</t>
-  </si>
-  <si>
-    <t>LFOK</t>
-  </si>
-  <si>
-    <t>Tours-Val de Loire</t>
-  </si>
-  <si>
-    <t>LFOT</t>
-  </si>
-  <si>
-    <t>Paris-Le Bourget</t>
-  </si>
-  <si>
-    <t>LFPB</t>
-  </si>
-  <si>
-    <t>Paris-Charles-de-Gaulle</t>
-  </si>
-  <si>
-    <t>LFPG</t>
-  </si>
-  <si>
-    <t>Toussus-le-Noble</t>
-  </si>
-  <si>
-    <t>LFPN</t>
-  </si>
-  <si>
-    <t>Paris-Orly</t>
-  </si>
-  <si>
-    <t>LFPO</t>
-  </si>
-  <si>
-    <t>Lille-Lesquin</t>
-  </si>
-  <si>
-    <t>LFQQ</t>
-  </si>
-  <si>
-    <t>Brest-Bretagne</t>
-  </si>
-  <si>
-    <t>LFRB</t>
-  </si>
-  <si>
-    <t>Dinard-Pleurtuit-Saint-Malo</t>
-  </si>
-  <si>
-    <t>LFRD</t>
-  </si>
-  <si>
-    <t>Deauville-Normandie</t>
-  </si>
-  <si>
-    <t>LFRG</t>
-  </si>
-  <si>
-    <t>Lorient-Lann Bihoué</t>
-  </si>
-  <si>
-    <t>LFRH</t>
-  </si>
-  <si>
-    <t>Caen-Carpiquet</t>
-  </si>
-  <si>
-    <t>LFRK</t>
-  </si>
-  <si>
-    <t>Rennes-Saint-Jacques</t>
-  </si>
-  <si>
-    <t>LFRN</t>
-  </si>
-  <si>
-    <t>Lannion</t>
-  </si>
-  <si>
-    <t>LFRO</t>
-  </si>
-  <si>
-    <t>Quimper-Pluguffan</t>
-  </si>
-  <si>
-    <t>LFRQ</t>
-  </si>
-  <si>
-    <t>Nantes-Atlantique</t>
-  </si>
-  <si>
-    <t>LFRS</t>
-  </si>
-  <si>
-    <t>Saint-Nazaire-Montoir</t>
-  </si>
-  <si>
-    <t>LFRZ</t>
-  </si>
-  <si>
-    <t>Bâle-Mulhouse</t>
-  </si>
-  <si>
-    <t>LFSB</t>
-  </si>
-  <si>
-    <t>Brive-Souillac</t>
-  </si>
-  <si>
-    <t>LFSL</t>
-  </si>
-  <si>
-    <t>Strasbourg-Entzheim</t>
-  </si>
-  <si>
-    <t>LFST</t>
-  </si>
-  <si>
-    <t>Hyères-Le Palyvestre</t>
-  </si>
-  <si>
-    <t>LFTH</t>
-  </si>
-  <si>
-    <t>Nîmes-Garons</t>
-  </si>
-  <si>
-    <t>LFTW</t>
-  </si>
-  <si>
-    <t>Athens</t>
-  </si>
-  <si>
-    <t>LGAV</t>
-  </si>
-  <si>
-    <t>Budapest/ Ferihegy</t>
-  </si>
-  <si>
-    <t>LHBP</t>
-  </si>
-  <si>
-    <t>Milan/ Malpensa</t>
-  </si>
-  <si>
-    <t>LIMC</t>
-  </si>
-  <si>
-    <t>Bergamo</t>
-  </si>
-  <si>
-    <t>LIME</t>
-  </si>
-  <si>
-    <t>Milan/ Linate</t>
-  </si>
-  <si>
-    <t>LIML</t>
-  </si>
-  <si>
-    <t>Venice</t>
-  </si>
-  <si>
-    <t>LIPZ</t>
-  </si>
-  <si>
-    <t>Rome/Fiumicino</t>
-  </si>
-  <si>
-    <t>LIRF</t>
-  </si>
-  <si>
-    <t>Ljubljana</t>
-  </si>
-  <si>
-    <t>LJLJ</t>
-  </si>
-  <si>
-    <t>Maribor</t>
-  </si>
-  <si>
-    <t>LJMB</t>
-  </si>
-  <si>
-    <t>Portorož</t>
-  </si>
-  <si>
-    <t>LJPZ</t>
-  </si>
-  <si>
-    <t>Karlovy Vary</t>
-  </si>
-  <si>
-    <t>LKKV</t>
-  </si>
-  <si>
-    <t>Ostrava</t>
-  </si>
-  <si>
-    <t>LKMT</t>
-  </si>
-  <si>
-    <t>Prague</t>
-  </si>
-  <si>
-    <t>LKPR</t>
-  </si>
-  <si>
-    <t>Brno-Tuřany</t>
-  </si>
-  <si>
-    <t>LKTB</t>
-  </si>
-  <si>
-    <t>LMML</t>
-  </si>
-  <si>
-    <t>Graz</t>
-  </si>
-  <si>
-    <t>LOWG</t>
-  </si>
-  <si>
-    <t>Innsbruck</t>
-  </si>
-  <si>
-    <t>LOWI</t>
-  </si>
-  <si>
-    <t>Klagenfurt</t>
-  </si>
-  <si>
-    <t>LOWK</t>
-  </si>
-  <si>
-    <t>Linz</t>
-  </si>
-  <si>
-    <t>LOWL</t>
-  </si>
-  <si>
-    <t>Salzburg</t>
-  </si>
-  <si>
-    <t>LOWS</t>
-  </si>
-  <si>
-    <t>Vienna</t>
-  </si>
-  <si>
-    <t>LOWW</t>
-  </si>
-  <si>
-    <t>Santa Maria</t>
-  </si>
-  <si>
-    <t>LPAZ</t>
-  </si>
-  <si>
-    <t>Cascais</t>
-  </si>
-  <si>
-    <t>LPCS</t>
-  </si>
-  <si>
-    <t>Flores</t>
-  </si>
-  <si>
-    <t>LPFL</t>
-  </si>
-  <si>
-    <t>Faro</t>
-  </si>
-  <si>
-    <t>LPFR</t>
-  </si>
-  <si>
-    <t>Horta</t>
-  </si>
-  <si>
-    <t>LPHR</t>
-  </si>
-  <si>
-    <t>Madeira</t>
-  </si>
-  <si>
-    <t>LPMA</t>
-  </si>
-  <si>
-    <t>Ponta Delgada</t>
-  </si>
-  <si>
-    <t>LPPD</t>
-  </si>
-  <si>
-    <t>Porto</t>
-  </si>
-  <si>
-    <t>LPPR</t>
-  </si>
-  <si>
-    <t>Porto Santo</t>
-  </si>
-  <si>
-    <t>LPPS</t>
-  </si>
-  <si>
-    <t>Lisbon</t>
-  </si>
-  <si>
-    <t>LPPT</t>
-  </si>
-  <si>
-    <t>Bucharest/ Băneasa</t>
-  </si>
-  <si>
-    <t>LRBS</t>
-  </si>
-  <si>
-    <t>Bucharest/ Otopeni</t>
-  </si>
-  <si>
-    <t>LROP</t>
-  </si>
-  <si>
-    <t>Geneva</t>
-  </si>
-  <si>
-    <t>LSGG</t>
-  </si>
-  <si>
-    <t>Zürich</t>
-  </si>
-  <si>
-    <t>LSZH</t>
-  </si>
-  <si>
-    <t>Bratislava</t>
-  </si>
-  <si>
-    <t>LZIB</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1313,8 @@
     <font>
       <u/>
       <sz val="9.0"/>
-      <color rgb="FF396EA2"/>
-      <name val="Calibri"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="9.0"/>
@@ -1471,7 +1471,7 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
@@ -1489,7 +1489,7 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -1566,33 +1566,33 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-    <col customWidth="1" min="2" max="2" width="19.71"/>
-    <col customWidth="1" min="3" max="3" width="16.43"/>
-    <col customWidth="1" min="4" max="4" width="16.71"/>
-    <col customWidth="1" min="5" max="5" width="11.86"/>
-    <col customWidth="1" min="6" max="6" width="11.57"/>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="17.25"/>
+    <col customWidth="1" min="3" max="3" width="14.38"/>
+    <col customWidth="1" min="4" max="4" width="14.63"/>
+    <col customWidth="1" min="5" max="5" width="10.38"/>
+    <col customWidth="1" min="6" max="6" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2252,21 +2252,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-    <col customWidth="1" min="2" max="2" width="37.0"/>
-    <col customWidth="1" min="3" max="3" width="11.71"/>
-    <col customWidth="1" min="4" max="4" width="16.0"/>
-    <col customWidth="1" min="5" max="5" width="15.0"/>
-    <col customWidth="1" min="6" max="6" width="17.43"/>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="32.38"/>
+    <col customWidth="1" min="3" max="3" width="10.25"/>
+    <col customWidth="1" min="4" max="4" width="14.0"/>
+    <col customWidth="1" min="5" max="5" width="13.13"/>
+    <col customWidth="1" min="6" max="6" width="15.25"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2923,7 +2923,7 @@
         <v>121</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D33" s="21">
         <f t="shared" si="1"/>
@@ -2941,10 +2941,10 @@
         <v>62</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D34" s="21" t="str">
         <f t="shared" si="1"/>
@@ -2962,10 +2962,10 @@
         <v>62</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D35" s="21" t="str">
         <f t="shared" si="1"/>
@@ -2983,10 +2983,10 @@
         <v>62</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D36" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3004,10 +3004,10 @@
         <v>62</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D37" s="21">
         <f t="shared" si="1"/>
@@ -3025,10 +3025,10 @@
         <v>62</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D38" s="21">
         <f t="shared" si="1"/>
@@ -3046,10 +3046,10 @@
         <v>48</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D39" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3067,10 +3067,10 @@
         <v>48</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D40" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3088,10 +3088,10 @@
         <v>48</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D41" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3109,10 +3109,10 @@
         <v>48</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D42" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3130,10 +3130,10 @@
         <v>39</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D43" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3151,10 +3151,10 @@
         <v>39</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D44" s="21">
         <f t="shared" si="1"/>
@@ -3172,10 +3172,10 @@
         <v>39</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D45" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3193,10 +3193,10 @@
         <v>29</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D46" s="21">
         <f t="shared" si="1"/>
@@ -3217,7 +3217,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D47" s="21">
         <f t="shared" si="1"/>
@@ -3235,10 +3235,10 @@
         <v>49</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D48" s="21">
         <f t="shared" si="1"/>
@@ -3256,10 +3256,10 @@
         <v>49</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D49" s="21">
         <f t="shared" si="1"/>
@@ -3277,10 +3277,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D50" s="21">
         <f t="shared" si="1"/>
@@ -3298,10 +3298,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D51" s="21">
         <f t="shared" si="1"/>
@@ -3319,10 +3319,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D52" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3340,10 +3340,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D53" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3361,10 +3361,10 @@
         <v>51</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D54" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3382,10 +3382,10 @@
         <v>51</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D55" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3403,10 +3403,10 @@
         <v>51</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D56" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3424,10 +3424,10 @@
         <v>51</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D57" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3445,10 +3445,10 @@
         <v>51</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D58" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3466,10 +3466,10 @@
         <v>51</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D59" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3487,10 +3487,10 @@
         <v>51</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C60" s="25" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D60" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3508,10 +3508,10 @@
         <v>51</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D61" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3529,10 +3529,10 @@
         <v>51</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D62" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3550,10 +3550,10 @@
         <v>51</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D63" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3571,10 +3571,10 @@
         <v>51</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D64" s="21">
         <f t="shared" si="1"/>
@@ -3592,10 +3592,10 @@
         <v>51</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D65" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3613,10 +3613,10 @@
         <v>51</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D66" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3634,10 +3634,10 @@
         <v>59</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D67" s="21">
         <f t="shared" si="1"/>
@@ -3655,10 +3655,10 @@
         <v>43</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D68" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3676,10 +3676,10 @@
         <v>43</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D69" s="21">
         <f t="shared" si="1"/>
@@ -3697,10 +3697,10 @@
         <v>43</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D70" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3718,10 +3718,10 @@
         <v>44</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D71" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3739,10 +3739,10 @@
         <v>44</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D72" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3760,10 +3760,10 @@
         <v>44</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D73" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3781,10 +3781,10 @@
         <v>44</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C74" s="25" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D74" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3802,10 +3802,10 @@
         <v>58</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D75" s="21">
         <f t="shared" si="1"/>
@@ -3823,10 +3823,10 @@
         <v>21</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C76" s="25" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D76" s="21">
         <f t="shared" si="1"/>
@@ -3844,10 +3844,10 @@
         <v>25</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C77" s="25" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D77" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3865,10 +3865,10 @@
         <v>25</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D78" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3886,10 +3886,10 @@
         <v>23</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C79" s="25" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D79" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3907,10 +3907,10 @@
         <v>58</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C80" s="25" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D80" s="21">
         <f t="shared" si="1"/>
@@ -3928,10 +3928,10 @@
         <v>58</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D81" s="21">
         <f t="shared" si="1"/>
@@ -3949,10 +3949,10 @@
         <v>58</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C82" s="25" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D82" s="21">
         <f t="shared" si="1"/>
@@ -3970,10 +3970,10 @@
         <v>58</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C83" s="25" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D83" s="21">
         <f t="shared" si="1"/>
@@ -3991,10 +3991,10 @@
         <v>33</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C84" s="25" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D84" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4012,10 +4012,10 @@
         <v>33</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D85" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4033,10 +4033,10 @@
         <v>33</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C86" s="25" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D86" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4054,10 +4054,10 @@
         <v>33</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C87" s="25" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D87" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4075,10 +4075,10 @@
         <v>33</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C88" s="25" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D88" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4096,10 +4096,10 @@
         <v>33</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C89" s="25" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D89" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4117,10 +4117,10 @@
         <v>33</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D90" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4138,10 +4138,10 @@
         <v>33</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C91" s="25" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D91" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4159,10 +4159,10 @@
         <v>33</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C92" s="25" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D92" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4180,10 +4180,10 @@
         <v>33</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C93" s="25" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D93" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4201,10 +4201,10 @@
         <v>33</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C94" s="25" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="D94" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4222,10 +4222,10 @@
         <v>33</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C95" s="25" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="D95" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4243,10 +4243,10 @@
         <v>33</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C96" s="25" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D96" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4264,10 +4264,10 @@
         <v>33</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C97" s="25" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D97" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4285,10 +4285,10 @@
         <v>33</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C98" s="25" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D98" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4306,10 +4306,10 @@
         <v>33</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C99" s="25" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D99" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4327,10 +4327,10 @@
         <v>33</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C100" s="25" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D100" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4348,10 +4348,10 @@
         <v>33</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C101" s="25" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D101" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4369,10 +4369,10 @@
         <v>33</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C102" s="25" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D102" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4390,10 +4390,10 @@
         <v>33</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C103" s="25" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D103" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4411,10 +4411,10 @@
         <v>33</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C104" s="25" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D104" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4432,10 +4432,10 @@
         <v>33</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C105" s="25" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D105" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4453,10 +4453,10 @@
         <v>33</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C106" s="25" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D106" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4474,10 +4474,10 @@
         <v>33</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C107" s="25" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D107" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4495,10 +4495,10 @@
         <v>33</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D108" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4516,10 +4516,10 @@
         <v>33</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="C109" s="25" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D109" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4537,10 +4537,10 @@
         <v>33</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C110" s="25" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D110" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4558,10 +4558,10 @@
         <v>33</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C111" s="25" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D111" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4579,10 +4579,10 @@
         <v>33</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="C112" s="25" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D112" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4600,10 +4600,10 @@
         <v>33</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C113" s="25" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="D113" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4621,10 +4621,10 @@
         <v>33</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="C114" s="25" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D114" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4642,10 +4642,10 @@
         <v>33</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C115" s="25" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D115" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4663,10 +4663,10 @@
         <v>33</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C116" s="25" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="D116" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4684,10 +4684,10 @@
         <v>33</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C117" s="25" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="D117" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4705,10 +4705,10 @@
         <v>33</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="C118" s="25" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D118" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4726,10 +4726,10 @@
         <v>33</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C119" s="25" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="D119" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4747,10 +4747,10 @@
         <v>33</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C120" s="25" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="D120" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4768,10 +4768,10 @@
         <v>33</v>
       </c>
       <c r="B121" s="25" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C121" s="25" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D121" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4789,10 +4789,10 @@
         <v>33</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C122" s="25" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="D122" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4810,10 +4810,10 @@
         <v>33</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C123" s="25" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D123" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4831,10 +4831,10 @@
         <v>33</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="C124" s="25" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="D124" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4852,10 +4852,10 @@
         <v>33</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="C125" s="25" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="D125" s="21">
         <f t="shared" si="1"/>
@@ -4873,10 +4873,10 @@
         <v>33</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C126" s="25" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D126" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4894,10 +4894,10 @@
         <v>33</v>
       </c>
       <c r="B127" s="25" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C127" s="25" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="D127" s="21">
         <f t="shared" si="1"/>
@@ -4915,10 +4915,10 @@
         <v>33</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="C128" s="25" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="D128" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4936,10 +4936,10 @@
         <v>33</v>
       </c>
       <c r="B129" s="25" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C129" s="25" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D129" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4957,10 +4957,10 @@
         <v>33</v>
       </c>
       <c r="B130" s="25" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="C130" s="25" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="D130" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4978,10 +4978,10 @@
         <v>33</v>
       </c>
       <c r="B131" s="25" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="C131" s="25" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="D131" s="21" t="str">
         <f t="shared" si="1"/>
@@ -4999,10 +4999,10 @@
         <v>33</v>
       </c>
       <c r="B132" s="25" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C132" s="25" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D132" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5020,10 +5020,10 @@
         <v>33</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C133" s="25" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="D133" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5041,10 +5041,10 @@
         <v>33</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C134" s="25" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="D134" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5062,10 +5062,10 @@
         <v>33</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C135" s="25" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D135" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5083,10 +5083,10 @@
         <v>33</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="C136" s="25" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D136" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5104,10 +5104,10 @@
         <v>33</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="C137" s="25" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="D137" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5125,10 +5125,10 @@
         <v>33</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C138" s="25" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D138" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5146,10 +5146,10 @@
         <v>33</v>
       </c>
       <c r="B139" s="25" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C139" s="25" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="D139" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5167,10 +5167,10 @@
         <v>33</v>
       </c>
       <c r="B140" s="25" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C140" s="25" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="D140" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5188,10 +5188,10 @@
         <v>33</v>
       </c>
       <c r="B141" s="25" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="C141" s="25" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="D141" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5209,10 +5209,10 @@
         <v>33</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C142" s="25" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="D142" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5230,10 +5230,10 @@
         <v>33</v>
       </c>
       <c r="B143" s="25" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C143" s="25" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D143" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5251,10 +5251,10 @@
         <v>37</v>
       </c>
       <c r="B144" s="25" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="C144" s="25" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D144" s="21">
         <f t="shared" si="1"/>
@@ -5272,10 +5272,10 @@
         <v>38</v>
       </c>
       <c r="B145" s="25" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C145" s="25" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="D145" s="21">
         <f t="shared" si="1"/>
@@ -5293,10 +5293,10 @@
         <v>41</v>
       </c>
       <c r="B146" s="25" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="C146" s="25" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="D146" s="21">
         <f t="shared" si="1"/>
@@ -5314,10 +5314,10 @@
         <v>41</v>
       </c>
       <c r="B147" s="25" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C147" s="25" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="D147" s="21">
         <f t="shared" si="1"/>
@@ -5335,10 +5335,10 @@
         <v>41</v>
       </c>
       <c r="B148" s="25" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C148" s="25" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D148" s="21">
         <f t="shared" si="1"/>
@@ -5356,10 +5356,10 @@
         <v>41</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C149" s="25" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="D149" s="21">
         <f t="shared" si="1"/>
@@ -5377,10 +5377,10 @@
         <v>41</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="C150" s="25" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D150" s="21">
         <f t="shared" si="1"/>
@@ -5398,10 +5398,10 @@
         <v>57</v>
       </c>
       <c r="B151" s="25" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="C151" s="25" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D151" s="21">
         <f t="shared" si="1"/>
@@ -5419,10 +5419,10 @@
         <v>57</v>
       </c>
       <c r="B152" s="25" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C152" s="25" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="D152" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5440,10 +5440,10 @@
         <v>57</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C153" s="25" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="D153" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5461,10 +5461,10 @@
         <v>27</v>
       </c>
       <c r="B154" s="25" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C154" s="25" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="D154" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5482,10 +5482,10 @@
         <v>27</v>
       </c>
       <c r="B155" s="25" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C155" s="25" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="D155" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5503,10 +5503,10 @@
         <v>27</v>
       </c>
       <c r="B156" s="25" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C156" s="25" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="D156" s="21">
         <f t="shared" si="1"/>
@@ -5524,10 +5524,10 @@
         <v>27</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="C157" s="25" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="D157" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5548,7 +5548,7 @@
         <v>47</v>
       </c>
       <c r="C158" s="25" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="D158" s="21">
         <f t="shared" si="1"/>
@@ -5566,10 +5566,10 @@
         <v>17</v>
       </c>
       <c r="B159" s="25" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="C159" s="25" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="D159" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5587,10 +5587,10 @@
         <v>17</v>
       </c>
       <c r="B160" s="25" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="C160" s="25" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="D160" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5608,10 +5608,10 @@
         <v>17</v>
       </c>
       <c r="B161" s="25" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C161" s="25" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D161" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5629,10 +5629,10 @@
         <v>17</v>
       </c>
       <c r="B162" s="25" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C162" s="25" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D162" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5650,10 +5650,10 @@
         <v>17</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="C163" s="25" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D163" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5671,10 +5671,10 @@
         <v>17</v>
       </c>
       <c r="B164" s="25" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C164" s="25" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="D164" s="21">
         <f t="shared" si="1"/>
@@ -5692,10 +5692,10 @@
         <v>53</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="C165" s="25" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="D165" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5713,10 +5713,10 @@
         <v>53</v>
       </c>
       <c r="B166" s="25" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="C166" s="25" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D166" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5734,10 +5734,10 @@
         <v>53</v>
       </c>
       <c r="B167" s="25" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="C167" s="25" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D167" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5755,10 +5755,10 @@
         <v>53</v>
       </c>
       <c r="B168" s="25" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C168" s="25" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="D168" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5776,10 +5776,10 @@
         <v>53</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C169" s="25" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="D169" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5797,10 +5797,10 @@
         <v>53</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="C170" s="25" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="D170" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5818,10 +5818,10 @@
         <v>53</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C171" s="25" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="D171" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5839,10 +5839,10 @@
         <v>53</v>
       </c>
       <c r="B172" s="25" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C172" s="25" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D172" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5860,10 +5860,10 @@
         <v>53</v>
       </c>
       <c r="B173" s="25" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="C173" s="25" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="D173" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5881,10 +5881,10 @@
         <v>53</v>
       </c>
       <c r="B174" s="25" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C174" s="25" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D174" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5902,10 +5902,10 @@
         <v>55</v>
       </c>
       <c r="B175" s="25" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="C175" s="25" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="D175" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5923,10 +5923,10 @@
         <v>55</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="C176" s="25" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="D176" s="21" t="str">
         <f t="shared" si="1"/>
@@ -5944,10 +5944,10 @@
         <v>60</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="C177" s="25" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="D177" s="21">
         <f t="shared" si="1"/>
@@ -5965,10 +5965,10 @@
         <v>60</v>
       </c>
       <c r="B178" s="25" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C178" s="25" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="D178" s="21">
         <f t="shared" si="1"/>
@@ -5986,10 +5986,10 @@
         <v>56</v>
       </c>
       <c r="B179" s="25" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="C179" s="25" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="D179" s="21" t="str">
         <f t="shared" si="1"/>
@@ -6011,33 +6011,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.57"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="8.0"/>
-    <col customWidth="1" min="4" max="4" width="113.57"/>
+    <col customWidth="1" min="1" max="1" width="9.25"/>
+    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="3" max="3" width="7.0"/>
+    <col customWidth="1" min="4" max="4" width="99.38"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="27" t="s">
-        <v>122</v>
+        <v>413</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>123</v>
+        <v>414</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>124</v>
+        <v>415</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>125</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -6045,27 +6045,27 @@
         <v>42779.0</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>126</v>
+        <v>417</v>
       </c>
       <c r="C2" s="31">
         <v>2016.0</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>127</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="32" t="s">
-        <v>128</v>
+        <v>419</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>129</v>
+        <v>420</v>
       </c>
       <c r="C3" s="32">
         <v>2016.0</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>130</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
@@ -6073,13 +6073,13 @@
         <v>42956.0</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>126</v>
+        <v>417</v>
       </c>
       <c r="C4" s="32">
         <v>2016.0</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>131</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">

</xml_diff>